<commit_message>
updated spreadsheet with RNA extraction notes
All samples from phase 2 have been extracted for RNA, the samples extracted by CM have been assessed for RNA quantity via qubit, those extracted on 5/17 by ST OC and AC have yet to be run on qubit.
</commit_message>
<xml_diff>
--- a/molecular/phase-2-data.xlsx
+++ b/molecular/phase-2-data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssdon\OneDrive\Documents\fish541_lab\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssdon\OneDrive\Documents\fish541_lab\molecular\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DCB939-75FA-439D-A82B-3764285C10B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CDDB49-3337-456B-9A45-C049F15EC3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="45">
   <si>
     <t>mussel-id</t>
   </si>
@@ -96,9 +96,6 @@
     <t>C11</t>
   </si>
   <si>
-    <t>note</t>
-  </si>
-  <si>
     <t>empty</t>
   </si>
   <si>
@@ -127,6 +124,42 @@
   </si>
   <si>
     <t>gill-tissue-RNA-id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yellow </t>
+  </si>
+  <si>
+    <t>RNA-note</t>
+  </si>
+  <si>
+    <t>qubit</t>
+  </si>
+  <si>
+    <t>sample-note</t>
+  </si>
+  <si>
+    <t>5/13 CM</t>
+  </si>
+  <si>
+    <t>5/13 CM disturbed pellet during 750ul transfer</t>
+  </si>
+  <si>
+    <t>5/13 CM small sample</t>
+  </si>
+  <si>
+    <t>5/17 AC</t>
+  </si>
+  <si>
+    <t>5/13 CM no sample?</t>
+  </si>
+  <si>
+    <t>5/17 ST</t>
+  </si>
+  <si>
+    <t>5/17 OC</t>
+  </si>
+  <si>
+    <t>5/17 ST not in spreadsheet originally</t>
   </si>
 </sst>
 </file>
@@ -168,11 +201,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -465,9 +502,11 @@
     <col min="5" max="5" width="10.59765625" customWidth="1"/>
     <col min="6" max="6" width="14.9296875" customWidth="1"/>
     <col min="7" max="7" width="15.265625" customWidth="1"/>
+    <col min="8" max="8" width="18.265625" customWidth="1"/>
+    <col min="9" max="9" width="9.06640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -487,13 +526,19 @@
         <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -512,10 +557,13 @@
         <v>50</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+        <v>33</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -536,8 +584,11 @@
       <c r="H3" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I3" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -558,8 +609,11 @@
       <c r="H4" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I4" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -580,10 +634,13 @@
         <v>5</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+        <v>29</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -604,8 +661,11 @@
       <c r="H6" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I6" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -626,8 +686,11 @@
       <c r="H7" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I7" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -648,10 +711,13 @@
         <v>5</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+        <v>29</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -674,8 +740,11 @@
       <c r="H9" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I9" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -696,8 +765,11 @@
       <c r="H10" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I10" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -718,10 +790,13 @@
         <v>5</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+        <v>30</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -742,10 +817,13 @@
         <v>60</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -766,10 +844,13 @@
         <v>61</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -790,10 +871,13 @@
         <v>62</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -814,10 +898,13 @@
         <v>63</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -838,10 +925,13 @@
         <v>64</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>101</v>
       </c>
@@ -862,10 +952,13 @@
         <v>66</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>102</v>
       </c>
@@ -886,10 +979,13 @@
         <v>67</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>103</v>
       </c>
@@ -910,10 +1006,13 @@
         <v>68</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>104</v>
       </c>
@@ -934,10 +1033,13 @@
         <v>69</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
@@ -960,10 +1062,13 @@
         <v>5</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>11</v>
       </c>
@@ -982,10 +1087,13 @@
         <v>80</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>12</v>
       </c>
@@ -1004,10 +1112,13 @@
         <v>81</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>13</v>
       </c>
@@ -1028,10 +1139,13 @@
         <v>5</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+        <v>29</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>14</v>
       </c>
@@ -1050,10 +1164,13 @@
         <v>83</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>15</v>
       </c>
@@ -1072,10 +1189,13 @@
         <v>5</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>16</v>
       </c>
@@ -1094,10 +1214,13 @@
         <v>85</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>17</v>
       </c>
@@ -1116,10 +1239,13 @@
         <v>86</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>18</v>
       </c>
@@ -1140,10 +1266,13 @@
         <v>88</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>19</v>
       </c>
@@ -1162,10 +1291,13 @@
         <v>87</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>20</v>
       </c>
@@ -1184,10 +1316,13 @@
         <v>89</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>111</v>
       </c>
@@ -1208,10 +1343,13 @@
         <v>82</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>5</v>
       </c>
@@ -1231,195 +1369,219 @@
         <v>5</v>
       </c>
       <c r="G33" s="1">
+        <v>70</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G34" s="1">
         <v>71</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A34" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G34" s="1">
+      <c r="H34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G35" s="1">
         <v>72</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A35" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G35" s="1">
+      <c r="H35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G36" s="1">
         <v>73</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G36" s="1">
+      <c r="H36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" s="1">
         <v>74</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A37" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G37" s="1">
+      <c r="H37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G38" s="1">
         <v>75</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A38" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G38" s="1">
+      <c r="H38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G39" s="1">
         <v>76</v>
       </c>
-      <c r="H38" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A39" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G39" s="1">
+      <c r="H39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G40" s="1">
         <v>77</v>
       </c>
-      <c r="H39" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A40" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="H40" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>5</v>
       </c>
@@ -1442,34 +1604,44 @@
         <v>5</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A43" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1">
-        <v>59.38</v>
-      </c>
-      <c r="G42" s="1">
-        <v>90</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A43" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>10</v>
@@ -1480,18 +1652,21 @@
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1">
-        <v>66.66</v>
+        <v>59.38</v>
       </c>
       <c r="G43" s="1">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>10</v>
@@ -1502,18 +1677,21 @@
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1">
-        <v>68.75</v>
+        <v>66.66</v>
       </c>
       <c r="G44" s="1">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>10</v>
@@ -1524,18 +1702,21 @@
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1">
-        <v>65.62</v>
+        <v>68.75</v>
       </c>
       <c r="G45" s="1">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>10</v>
@@ -1546,18 +1727,21 @@
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1">
-        <v>61.45</v>
+        <v>65.62</v>
       </c>
       <c r="G46" s="1">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>10</v>
@@ -1568,18 +1752,21 @@
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1">
-        <v>63.54</v>
+        <v>61.45</v>
       </c>
       <c r="G47" s="1">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>10</v>
@@ -1590,18 +1777,21 @@
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1">
-        <v>47.92</v>
+        <v>63.54</v>
       </c>
       <c r="G48" s="1">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>10</v>
@@ -1612,18 +1802,21 @@
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1">
-        <v>55.23</v>
+        <v>47.92</v>
       </c>
       <c r="G49" s="1">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>10</v>
@@ -1634,18 +1827,21 @@
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1">
-        <v>61.47</v>
+        <v>55.23</v>
       </c>
       <c r="G50" s="1">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>10</v>
@@ -1656,18 +1852,21 @@
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1">
-        <v>55.2</v>
+        <v>61.47</v>
       </c>
       <c r="G51" s="1">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>10</v>
@@ -1678,17 +1877,49 @@
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1">
+        <v>55.2</v>
+      </c>
+      <c r="G52" s="1">
+        <v>99</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A53" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1">
         <v>62.5</v>
       </c>
-      <c r="G52" s="1">
+      <c r="G53" s="1">
         <v>100</v>
       </c>
-      <c r="H52" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="H53" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H54" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>